<commit_message>
incluindo o cógigo js do inputPath
</commit_message>
<xml_diff>
--- a/assets/archives/Rota.xlsx
+++ b/assets/archives/Rota.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
   <si>
     <t>Roteiro</t>
   </si>
@@ -49,9 +49,6 @@
     <t>Total de Notas:</t>
   </si>
   <si>
-    <t>Total da carga (Kg)</t>
-  </si>
-  <si>
     <t>domingo</t>
   </si>
   <si>
@@ -92,6 +89,15 @@
   </si>
   <si>
     <t>AV. DUQUE DE CAXIAS,782</t>
+  </si>
+  <si>
+    <t>putAKeepAreYou</t>
+  </si>
+  <si>
+    <t>nada para nada</t>
+  </si>
+  <si>
+    <t>´pourrra</t>
   </si>
 </sst>
 </file>
@@ -458,7 +464,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -509,31 +515,31 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>18</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>19</v>
-      </c>
-      <c r="I2" t="s">
-        <v>20</v>
       </c>
       <c r="J2">
         <v>8</v>
@@ -541,31 +547,31 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
       <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
         <v>21</v>
       </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" t="s">
         <v>22</v>
-      </c>
-      <c r="H3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" t="s">
-        <v>23</v>
       </c>
       <c r="J3">
         <v>8</v>
@@ -573,31 +579,31 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
       <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" t="s">
         <v>24</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" t="s">
-        <v>25</v>
       </c>
       <c r="J4">
         <v>8</v>
@@ -643,7 +649,7 @@
     </row>
     <row r="7" spans="1:10" ht="24.95" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B7" s="3"/>
     </row>

</xml_diff>

<commit_message>
Criação da página ramais.tml
</commit_message>
<xml_diff>
--- a/assets/archives/Rota.xlsx
+++ b/assets/archives/Rota.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t xml:space="preserve">DIA</t>
   </si>
@@ -46,31 +46,34 @@
     <t xml:space="preserve">26/02/22</t>
   </si>
   <si>
+    <t xml:space="preserve">vicente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARCOVITA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07:00 ÀS 13:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.9774-2208</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VICENTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BEBERIBE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13:00 ÀS 19:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.9806-5558</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOMINGO</t>
+  </si>
+  <si>
     <t xml:space="preserve">CARLOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARCOVITA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">07:00 ÀS 13:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.9774-2208</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VICENTE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BEBERIBE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13:00 ÀS 19:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.9806-5558</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DOMINGO</t>
   </si>
   <si>
     <t xml:space="preserve">07:00 ÀS 14:00</t>
@@ -209,11 +212,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -242,10 +245,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -255,11 +258,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="40"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -281,9 +284,6 @@
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0"/>
-      <c r="H1" s="0"/>
-      <c r="I1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
@@ -304,9 +304,6 @@
       <c r="F2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="0"/>
-      <c r="H2" s="0"/>
-      <c r="I2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
@@ -327,9 +324,6 @@
       <c r="F3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="0"/>
-      <c r="H3" s="0"/>
-      <c r="I3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
@@ -339,20 +333,17 @@
         <v>7</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="0"/>
-      <c r="H4" s="0"/>
-      <c r="I4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7"/>
@@ -361,25 +352,8 @@
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
-      <c r="G5" s="0"/>
-      <c r="H5" s="0"/>
-      <c r="I5" s="0"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F6" s="1"/>
-      <c r="G6" s="0"/>
-      <c r="H6" s="0"/>
-      <c r="I6" s="0"/>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F7" s="1"/>
-      <c r="G7" s="0"/>
-      <c r="H7" s="0"/>
-      <c r="I7" s="0"/>
-    </row>
-    <row r="8" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F8" s="1"/>
-    </row>
+    </row>
+    <row r="8" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Modificação da sessão Team e adição de estilo css na sessão Ramais
</commit_message>
<xml_diff>
--- a/assets/archives/Rota.xlsx
+++ b/assets/archives/Rota.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t xml:space="preserve">DIA</t>
   </si>
@@ -43,40 +43,43 @@
     <t xml:space="preserve">SÁBADO</t>
   </si>
   <si>
-    <t xml:space="preserve">26/02/22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vicente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARCOVITA</t>
+    <t xml:space="preserve">03/06/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alexandre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HOME OFFICE</t>
   </si>
   <si>
     <t xml:space="preserve">07:00 ÀS 13:00</t>
   </si>
   <si>
+    <t xml:space="preserve">9.8209-1766</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tamires</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13:00 ÀS 19:00</t>
+  </si>
+  <si>
     <t xml:space="preserve">9.9774-2208</t>
   </si>
   <si>
-    <t xml:space="preserve">VICENTE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BEBERIBE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13:00 ÀS 19:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.9806-5558</t>
-  </si>
-  <si>
     <t xml:space="preserve">DOMINGO</t>
   </si>
   <si>
-    <t xml:space="preserve">CARLOS</t>
+    <t xml:space="preserve">04/06/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vicente</t>
   </si>
   <si>
     <t xml:space="preserve">07:00 ÀS 14:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.8116-2088</t>
   </si>
 </sst>
 </file>
@@ -241,17 +244,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E9:E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="12.93"/>
@@ -261,8 +264,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="40"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -316,21 +318,21 @@
         <v>12</v>
       </c>
       <c r="D3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>7</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>17</v>
@@ -342,7 +344,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>